<commit_message>
Updated(modified, renamed) Tables and Supplementary Tables
</commit_message>
<xml_diff>
--- a/Supplementary_files/Supplementary_Table_04.xlsx
+++ b/Supplementary_files/Supplementary_Table_04.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Comparison with other CoVs" sheetId="1" r:id="rId1"/>
+    <sheet name="Count of ZAP-binding motifs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="206">
   <si>
     <t>seq_id</t>
   </si>
@@ -86,6 +86,42 @@
   </si>
   <si>
     <t>match_score_for_conserved_stretch_11</t>
+  </si>
+  <si>
+    <t>cs_01_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_02_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_03_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_04_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_05_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_06_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_07_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_08_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_09_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_10_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>cs_11_zap_motifs_count</t>
+  </si>
+  <si>
+    <t>total_zap_count</t>
   </si>
   <si>
     <t>MN908947.3</t>
@@ -953,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:37">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1032,49 +1068,85 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:37">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="K2" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="M2" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="N2" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="O2">
         <v>100</v>
@@ -1109,49 +1181,85 @@
       <c r="Y2">
         <v>100</v>
       </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:37">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="L3" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="M3" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="N3" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="O3">
         <v>20.86330935251799</v>
@@ -1186,49 +1294,85 @@
       <c r="Y3">
         <v>41.17647058823529</v>
       </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:37">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="H4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="I4" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="K4" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="L4" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="M4" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="N4" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="O4">
         <v>20.14388489208633</v>
@@ -1263,49 +1407,85 @@
       <c r="Y4">
         <v>40.19607843137255</v>
       </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:37">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="I5" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="L5" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="M5" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="N5" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="O5">
         <v>34.53237410071942</v>
@@ -1340,49 +1520,85 @@
       <c r="Y5">
         <v>47.05882352941176</v>
       </c>
+      <c r="Z5">
+        <v>4</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:37">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="I6" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="J6" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K6" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="L6" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="M6" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="N6" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="O6">
         <v>34.53237410071942</v>
@@ -1417,49 +1633,85 @@
       <c r="Y6">
         <v>47.05882352941176</v>
       </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:37">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="I7" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="J7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="K7" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="L7" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="M7" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="N7" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="O7">
         <v>84.17266187050359</v>
@@ -1494,49 +1746,85 @@
       <c r="Y7">
         <v>93.13725490196079</v>
       </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:37">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="I8" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="J8" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="L8" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="M8" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="N8" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="O8">
         <v>30.93525179856115</v>
@@ -1571,49 +1859,85 @@
       <c r="Y8">
         <v>39.21568627450981</v>
       </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:37">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="I9" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="K9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="L9" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="M9" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="N9" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="O9">
         <v>35.97122302158273</v>
@@ -1648,49 +1972,85 @@
       <c r="Y9">
         <v>50.98039215686274</v>
       </c>
+      <c r="Z9">
+        <v>2</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>2</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>12</v>
+      </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:37">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="J10" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="K10" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="L10" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="M10" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="N10" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="O10">
         <v>39.56834532374101</v>
@@ -1725,49 +2085,85 @@
       <c r="Y10">
         <v>54.90196078431373</v>
       </c>
+      <c r="Z10">
+        <v>3</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:37">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="J11" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="K11" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="L11" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="M11" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="N11" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="O11">
         <v>33.81294964028777</v>
@@ -1802,49 +2198,85 @@
       <c r="Y11">
         <v>52.94117647058824</v>
       </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>2</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>5</v>
+      </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:37">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H12" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="J12" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="K12" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="L12" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="M12" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="N12" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="O12">
         <v>97.12230215827337</v>
@@ -1879,49 +2311,85 @@
       <c r="Y12">
         <v>99.01960784313727</v>
       </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:37">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="I13" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="J13" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="K13" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="L13" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="M13" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="N13" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="O13">
         <v>84.89208633093526</v>
@@ -1956,49 +2424,85 @@
       <c r="Y13">
         <v>94.11764705882352</v>
       </c>
+      <c r="Z13">
+        <v>2</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>4</v>
+      </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:37">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="I14" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="J14" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="K14" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="L14" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="M14" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="N14" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="O14">
         <v>26.61870503597122</v>
@@ -2033,49 +2537,85 @@
       <c r="Y14">
         <v>35.29411764705883</v>
       </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>2</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>3</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>7</v>
+      </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:37">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="H15" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="I15" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="J15" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="K15" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="L15" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="M15" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="N15" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="O15">
         <v>56.11510791366906</v>
@@ -2109,6 +2649,42 @@
       </c>
       <c r="Y15">
         <v>67.64705882352942</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>2</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>4</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>2</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15">
+        <v>1</v>
+      </c>
+      <c r="AK15">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>